<commit_message>
DMS: Translate Store Export and ExportTemplate
</commit_message>
<xml_diff>
--- a/DMS/Templates/Store_Template.xlsx
+++ b/DMS/Templates/Store_Template.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80E2156-3173-4D5C-A458-D6450B6B35EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492D5F4C-7493-484F-9DD4-37C647CAA903}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Store" sheetId="1" r:id="rId1"/>
-    <sheet name="Org" sheetId="2" r:id="rId2"/>
-    <sheet name="ParentStore" sheetId="6" r:id="rId3"/>
-    <sheet name="StoreType" sheetId="7" r:id="rId4"/>
-    <sheet name="StoreGroup" sheetId="8" r:id="rId5"/>
-    <sheet name="Province" sheetId="12" r:id="rId6"/>
-    <sheet name="District" sheetId="11" r:id="rId7"/>
-    <sheet name="Ward" sheetId="10" r:id="rId8"/>
+    <sheet name="Đại lý" sheetId="1" r:id="rId1"/>
+    <sheet name="Đơn vị tổ chức" sheetId="2" r:id="rId2"/>
+    <sheet name="Đại lý cha" sheetId="6" r:id="rId3"/>
+    <sheet name="Loại đại lý" sheetId="7" r:id="rId4"/>
+    <sheet name="Nhóm đại lý" sheetId="8" r:id="rId5"/>
+    <sheet name="Tỉnh, Thành phố" sheetId="12" r:id="rId6"/>
+    <sheet name="Quận, Huyện" sheetId="11" r:id="rId7"/>
+    <sheet name="Phường, Xã" sheetId="10" r:id="rId8"/>
     <sheet name="Quy tac import" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Store!$E$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Đại lý'!$E$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -187,7 +187,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -195,7 +195,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -216,7 +216,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -604,33 +604,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="3" customWidth="1"/>
-    <col min="2" max="3" width="12.25" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="12.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="27" style="3" customWidth="1"/>
     <col min="5" max="5" width="29" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.75" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.125" style="3" customWidth="1"/>
-    <col min="8" max="10" width="16.75" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="13.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="3" customWidth="1"/>
+    <col min="8" max="10" width="16.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="3" customWidth="1"/>
+    <col min="12" max="13" width="13.140625" style="3" customWidth="1"/>
     <col min="14" max="14" width="16" style="3" customWidth="1"/>
-    <col min="15" max="19" width="13.75" style="3" customWidth="1"/>
-    <col min="20" max="20" width="13.625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="16.125" style="3" customWidth="1"/>
-    <col min="22" max="22" width="18.625" style="3" customWidth="1"/>
-    <col min="23" max="24" width="20.75" style="3" customWidth="1"/>
-    <col min="25" max="25" width="19.375" style="3" customWidth="1"/>
-    <col min="26" max="26" width="17.375" style="3" customWidth="1"/>
-    <col min="27" max="16384" width="9.125" style="3"/>
+    <col min="15" max="19" width="13.7109375" style="3" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" style="3" customWidth="1"/>
+    <col min="23" max="24" width="20.7109375" style="3" customWidth="1"/>
+    <col min="25" max="25" width="19.42578125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" style="3" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -738,15 +738,15 @@
       <selection activeCell="A2" sqref="A2:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.25" customWidth="1"/>
-    <col min="2" max="2" width="30.75" customWidth="1"/>
-    <col min="3" max="3" width="27.875" customWidth="1"/>
-    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -754,22 +754,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -783,18 +783,18 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.25" customWidth="1"/>
-    <col min="2" max="2" width="30.25" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="41.875" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -808,22 +808,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -840,13 +840,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.125" customWidth="1"/>
-    <col min="2" max="2" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -854,22 +854,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -885,13 +885,13 @@
       <selection activeCell="A2" sqref="A2:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.625" customWidth="1"/>
-    <col min="2" max="2" width="46.75" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -899,22 +899,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -926,18 +926,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.25" customWidth="1"/>
-    <col min="2" max="2" width="47.875" customWidth="1"/>
-    <col min="3" max="3" width="31.875" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -945,22 +945,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -976,14 +976,14 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="33.875" customWidth="1"/>
-    <col min="3" max="3" width="28.625" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -994,22 +994,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1025,15 +1025,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-    <col min="2" max="2" width="36.875" customWidth="1"/>
-    <col min="3" max="3" width="25.875" customWidth="1"/>
-    <col min="4" max="4" width="30.875" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -1060,15 +1060,15 @@
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.125" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="9" max="9" width="20.625" customWidth="1"/>
-    <col min="10" max="10" width="27.375" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>32</v>
       </c>
@@ -1081,7 +1081,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -1092,7 +1092,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1103,7 +1103,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1114,7 +1114,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1125,7 +1125,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1136,7 +1136,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1147,7 +1147,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1158,7 +1158,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1169,7 +1169,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1180,7 +1180,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1191,7 +1191,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1202,7 +1202,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1213,7 +1213,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1224,7 +1224,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1235,7 +1235,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1246,7 +1246,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1257,7 +1257,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1268,7 +1268,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1279,7 +1279,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1290,7 +1290,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -1301,7 +1301,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -1312,7 +1312,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -1323,7 +1323,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -1334,7 +1334,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -1345,7 +1345,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -1356,7 +1356,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -1367,7 +1367,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -1378,7 +1378,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>

</xml_diff>